<commit_message>
wrote a lot in the documentation and other documents
</commit_message>
<xml_diff>
--- a/docs/API Endpoints.xlsx
+++ b/docs/API Endpoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lshut\Documents\Coding\jukestack_luis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C304E744-945F-46FC-93EB-323A97420258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51747EA-DC99-4B5E-B204-0C98718ED264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{757173FE-E8F1-4E48-97BE-10049B454DB7}"/>
+    <workbookView xWindow="-28920" yWindow="-1905" windowWidth="29040" windowHeight="17520" xr2:uid="{757173FE-E8F1-4E48-97BE-10049B454DB7}"/>
   </bookViews>
   <sheets>
     <sheet name="API Endpoints" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
   <si>
     <t>/api</t>
   </si>
@@ -147,9 +147,6 @@
     <t>List all users</t>
   </si>
   <si>
-    <t>/admin/users/{id}/lend</t>
-  </si>
-  <si>
     <t>List a users borrowed songs</t>
   </si>
   <si>
@@ -163,6 +160,30 @@
   </si>
   <si>
     <t>Return a users lend by lendId</t>
+  </si>
+  <si>
+    <t>/auth/sendVerify</t>
+  </si>
+  <si>
+    <t>Send verification email</t>
+  </si>
+  <si>
+    <t>/auth/verifyEmail</t>
+  </si>
+  <si>
+    <t>Verify email via tokenized link</t>
+  </si>
+  <si>
+    <t>/admin/users/{email}/lend</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Implemented</t>
+  </si>
+  <si>
+    <t>Response</t>
   </si>
 </sst>
 </file>
@@ -206,9 +227,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,20 +627,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D747BA-E446-4A84-986B-7B4C08CFB652}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -628,10 +653,13 @@
         <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -644,11 +672,14 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>201</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -661,11 +692,14 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -678,11 +712,14 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>200</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -695,11 +732,14 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -712,11 +752,14 @@
       <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>201</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -729,11 +772,14 @@
       <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>200</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -746,11 +792,14 @@
       <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>201</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -763,173 +812,243 @@
       <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>201</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="E10">
+        <v>200</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11">
+        <v>302</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12">
+        <v>200</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>33</v>
       </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="E13">
+        <v>200</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="E14">
+        <v>200</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>29</v>
       </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>200</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="E16">
+        <v>200</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17">
+        <v>200</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18">
+        <v>200</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
         <v>39</v>
       </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E19">
+        <v>200</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
         <v>40</v>
       </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="E20">
+        <v>200</v>
+      </c>
+      <c r="F20" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E27:E1048576 E2:E18">
+  <conditionalFormatting sqref="F2:F20 F29:F1048576">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>E2="Fully Implemented"</formula>
+      <formula>F2="Fully Implemented"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>E2="POC / MVP"</formula>
+      <formula>F2="POC / MVP"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>E2="Not Implemented"</formula>
+      <formula>F2="Not Implemented"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -941,13 +1060,13 @@
           <x14:formula1>
             <xm:f>util!$A$4:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C10 C28:C34 C14</xm:sqref>
+          <xm:sqref>C2:C12 C30:C36 C16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{806311F3-9564-4E1D-9F96-187326C63E67}">
           <x14:formula1>
             <xm:f>util!$C$4:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E10 E28:E34 E12:E18</xm:sqref>
+          <xm:sqref>F2:F12 F30:F36 F14:F20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>